<commit_message>
remove ioutil and add a new test/EmptyWorkbook.xlsx
Change-Id: I04479f92c559e4bbfa5e81d5698389122c90743c
</commit_message>
<xml_diff>
--- a/test/EmptyWorkbook.xlsx
+++ b/test/EmptyWorkbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bytedance/go/src/github.com/qax-os/excelize/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bytedance/go/src/github.com/jianxinhou/excelize/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21C902BB-1FCC-6346-A06A-0D4AFAA95CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7B91569-73A5-6C46-9A0C-BAD16CD943F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5080" yWindow="1800" windowWidth="28240" windowHeight="17440" xr2:uid="{36D07BA3-FCE3-E040-B3A3-F02B07BE3BE9}"/>
+    <workbookView xWindow="5080" yWindow="1800" windowWidth="28240" windowHeight="17440" xr2:uid="{A58F1008-83DA-A94D-9B7F-EF139595013D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,12 +391,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBF42FB-3088-D241-951B-E4E1B96E2AC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB197FAA-E2B9-8E41-B421-AA0AB7028FF7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>

</xml_diff>